<commit_message>
v1.0.3 Liste Route next
</commit_message>
<xml_diff>
--- a/to-do.xlsx
+++ b/to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITU\S6\Stage\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F633848-DD29-4A71-BAB8-8D1334CDA7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A995BC-5D42-4BFE-9B72-20DA969197A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8991ED85-435A-406D-9B42-8647D9730187}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="60">
   <si>
     <t>Nom :</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Nouvelle Portion</t>
   </si>
   <si>
-    <t>Liste Portion</t>
-  </si>
-  <si>
     <t>Avancement Total</t>
   </si>
   <si>
@@ -187,6 +184,27 @@
   </si>
   <si>
     <t>Page d'erreur</t>
+  </si>
+  <si>
+    <t>Liste Route</t>
+  </si>
+  <si>
+    <t>Export Excel</t>
+  </si>
+  <si>
+    <t>Nouvel Etat</t>
+  </si>
+  <si>
+    <t>Etat Route</t>
+  </si>
+  <si>
+    <t>Update Etat</t>
+  </si>
+  <si>
+    <t>Liste Etat</t>
+  </si>
+  <si>
+    <t>Liste Portion par route</t>
   </si>
 </sst>
 </file>
@@ -252,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AB2488C-A8B7-4115-A932-687B7139B560}" name="Table1" displayName="Table1" ref="A4:H59" totalsRowShown="0">
-  <autoFilter ref="A4:H59" xr:uid="{6AB2488C-A8B7-4115-A932-687B7139B560}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AB2488C-A8B7-4115-A932-687B7139B560}" name="Table1" displayName="Table1" ref="A4:H68" totalsRowShown="0">
+  <autoFilter ref="A4:H68" xr:uid="{6AB2488C-A8B7-4115-A932-687B7139B560}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{19ED5805-81D6-43FF-BC0E-44BBDC76AB16}" name="Catégorie"/>
     <tableColumn id="2" xr3:uid="{50E49B5F-158F-4CD4-93A3-9A78ED14BCB9}" name="Taches"/>
@@ -569,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF842E8-387E-4A80-91B0-664FA38FE2A4}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -638,10 +656,10 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
@@ -663,10 +681,10 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
@@ -679,38 +697,38 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="e">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="e">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -732,13 +750,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -757,10 +775,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -779,15 +797,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -809,13 +827,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -834,10 +852,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -915,7 +933,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -993,15 +1011,18 @@
         <v>19</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
       </c>
       <c r="F19">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1012,18 +1033,21 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
       </c>
       <c r="F20">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1037,48 +1061,54 @@
         <v>18</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
       </c>
       <c r="F21">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
       </c>
       <c r="F22">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>30</v>
@@ -1094,90 +1124,102 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D24">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
       </c>
       <c r="F24">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
       </c>
       <c r="F25">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D26">
-        <v>30</v>
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>12</v>
       </c>
       <c r="F26">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D27">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
       </c>
       <c r="F27">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,21 +1227,24 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>17</v>
       </c>
       <c r="F28">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,21 +1252,24 @@
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
       </c>
       <c r="F29">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,21 +1277,24 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E30">
+        <v>31</v>
       </c>
       <c r="F30">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,7 +1302,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -1259,13 +1310,16 @@
       <c r="D31">
         <v>10</v>
       </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
       <c r="F31">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G31" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1273,7 +1327,7 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -1295,10 +1349,10 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33">
         <v>30</v>
@@ -1314,20 +1368,20 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F34">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G34" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1336,13 +1390,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D35">
         <v>30</v>
@@ -1358,20 +1412,20 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F36">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G36" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1380,20 +1434,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F37">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G37" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1402,13 +1456,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D38">
         <v>30</v>
@@ -1424,20 +1478,20 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D39">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F39">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G39" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1446,20 +1500,20 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F40">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G40" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1468,13 +1522,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D41">
         <v>30</v>
@@ -1490,20 +1544,20 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D42">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F42">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G42" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1515,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
@@ -1537,10 +1591,10 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44">
         <v>30</v>
@@ -1559,17 +1613,17 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F45">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G45" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1581,17 +1635,17 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D46">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="F46">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="G46" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1600,13 +1654,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -1622,20 +1676,20 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
       </c>
       <c r="D48">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F48">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G48" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1644,10 +1698,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
@@ -1666,20 +1720,20 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D50">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F50">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G50" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1688,20 +1742,20 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D51">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F51">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G51" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1710,10 +1764,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
@@ -1732,13 +1786,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53">
         <v>30</v>
@@ -1754,20 +1808,20 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D54">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="F54">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G54" s="1">
         <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
@@ -1776,100 +1830,310 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
         <v>43</v>
       </c>
       <c r="D55">
+        <v>120</v>
+      </c>
+      <c r="F55">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>120</v>
+      </c>
+      <c r="G55" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56">
+        <v>30</v>
+      </c>
+      <c r="F56">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>30</v>
+      </c>
+      <c r="G56" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57">
+        <v>40</v>
+      </c>
+      <c r="F57">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>40</v>
+      </c>
+      <c r="G57" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58">
+        <v>30</v>
+      </c>
+      <c r="F58">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>30</v>
+      </c>
+      <c r="G58" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59">
         <v>60</v>
       </c>
-      <c r="F55">
+      <c r="F59">
         <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
         <v>60</v>
       </c>
-      <c r="G55" s="1">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F56">
-        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="1" t="e">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F57">
-        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="1" t="e">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F58">
-        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="1" t="e">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F59">
-        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="1" t="e">
-        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
-        <v>#DIV/0!</v>
+      <c r="G59" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60">
+        <v>60</v>
+      </c>
+      <c r="F60">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>60</v>
+      </c>
+      <c r="G60" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61">
+        <v>30</v>
+      </c>
+      <c r="F61">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>30</v>
+      </c>
+      <c r="G61" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62">
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>30</v>
+      </c>
+      <c r="G62" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63">
-        <f>SUM(Table1[Estimation (en min)])</f>
-        <v>1370</v>
+        <v>35</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63">
+        <v>20</v>
+      </c>
+      <c r="F63">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>20</v>
+      </c>
+      <c r="G63" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64">
+        <v>60</v>
+      </c>
+      <c r="F64">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>60</v>
+      </c>
+      <c r="G64" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65">
+        <v>120</v>
+      </c>
+      <c r="F65">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>120</v>
+      </c>
+      <c r="G65" s="1">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="1" t="e">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="1" t="e">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f>Table1[[#This Row],[Estimation (en min)]]-Table1[[#This Row],[Temps passé(en min)]]</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="1" t="e">
+        <f>Table1[[#This Row],[Temps passé(en min)]]/(Table1[[#This Row],[Temps passé(en min)]]+Table1[[#This Row],[Rest à faire (en min)]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <f>SUM(Table1[Estimation (en min)])</f>
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73">
+        <f>SUM(Table1[Temps passé(en min)])</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>27</v>
       </c>
-      <c r="B64">
-        <f>SUM(Table1[Temps passé(en min)])</f>
-        <v>161</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65">
+      <c r="B74">
         <f>SUM(Table1[Rest à faire (en min)])</f>
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" s="1">
-        <f>B64/(B64+B65)</f>
-        <v>0.11751824817518249</v>
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="1">
+        <f>B73/(B73+B74)</f>
+        <v>0.18566978193146416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>